<commit_message>
add danger log and update excel
</commit_message>
<xml_diff>
--- a/hw1_requirements.xlsx
+++ b/hw1_requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmrogers/Work/Teaching/ece568_s2019/homework/hw1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lintingxuan/Desktop/hw1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D75D6A-2EE1-104A-B584-697538A4DDD1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29E48C1-70A1-0C43-BB4F-D07137EB2B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="460" windowWidth="20120" windowHeight="15900" xr2:uid="{845B1E4D-506C-FC44-903E-E3158AE804D8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" xr2:uid="{845B1E4D-506C-FC44-903E-E3158AE804D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>Requirement</t>
   </si>
@@ -54,62 +54,84 @@
     <t>User should be able to register as a driver by entering their personal &amp; vehicle info</t>
   </si>
   <si>
+    <t>A ride owner should be able to edit the requested attributes of a ride until that ride is confirmed</t>
+  </si>
+  <si>
+    <t>User should be able to view all ride details for any open ride they belong to</t>
+  </si>
+  <si>
+    <t>User should be able to view all ride details + driver and vehicle details for any confirmed ride they belong to</t>
+  </si>
+  <si>
+    <t>User should be able to join a ride returned in a search as described in requirement #13</t>
+  </si>
+  <si>
+    <t>A registered driver should be able to search for open ride requests (filtered by the driver's vehicle capacity and type / special info, if applicable)</t>
+  </si>
+  <si>
+    <t>User should be able to make a selection to edit any open ride they belong to</t>
+  </si>
+  <si>
+    <t>An email should be sent to the owner and any sharers of a ride once it is confirmed by a driver</t>
+  </si>
+  <si>
+    <t>A registered driver should be able to mark a selected ride (returned from a search as described in requirement #15) as confirmed (thus claiming and starting the ride)</t>
+  </si>
+  <si>
+    <t>A driver should be able to see a list of their confirmed rides</t>
+  </si>
+  <si>
+    <t>A driver should be able to select a confirmed ride and view all of the ride details</t>
+  </si>
+  <si>
+    <t>A driver should be able to edit a confirmed ride for the purpose of marking it complete after the ride is over</t>
+  </si>
+  <si>
+    <t>User should be able to submit a ride request by specifying the required and any combination of the optional info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User should be able to make a selection to view any non-complete ride they belong to</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User should be able to search for sharable, open ride requests (by destination, arrival window, and # of passengers)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">User should be able to view and edit their driver status as well as personal &amp; vehicle info </t>
-  </si>
-  <si>
-    <t>User should be able to submit a ride request by specifying the required and any combination of the optional info</t>
-  </si>
-  <si>
-    <t>A ride owner should be able to edit the requested attributes of a ride until that ride is confirmed</t>
-  </si>
-  <si>
-    <t>User should be able to view all ride details for any open ride they belong to</t>
-  </si>
-  <si>
-    <t>User should be able to view all ride details + driver and vehicle details for any confirmed ride they belong to</t>
-  </si>
-  <si>
-    <t>User should be able to search for sharable, open ride requests (by destination, arrival window, and # of passengers)</t>
-  </si>
-  <si>
-    <t>User should be able to join a ride returned in a search as described in requirement #13</t>
-  </si>
-  <si>
-    <t>A registered driver should be able to search for open ride requests (filtered by the driver's vehicle capacity and type / special info, if applicable)</t>
-  </si>
-  <si>
-    <t>User should be able to make a selection to view any non-complete ride they belong to</t>
-  </si>
-  <si>
-    <t>User should be able to make a selection to edit any open ride they belong to</t>
-  </si>
-  <si>
-    <t>An email should be sent to the owner and any sharers of a ride once it is confirmed by a driver</t>
-  </si>
-  <si>
-    <t>A registered driver should be able to mark a selected ride (returned from a search as described in requirement #15) as confirmed (thus claiming and starting the ride)</t>
-  </si>
-  <si>
-    <t>A driver should be able to see a list of their confirmed rides</t>
-  </si>
-  <si>
-    <t>A driver should be able to select a confirmed ride and view all of the ride details</t>
-  </si>
-  <si>
-    <t>A driver should be able to edit a confirmed ride for the purpose of marking it complete after the ride is over</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體 (本文)"/>
+      <family val="1"/>
+      <charset val="136"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,14 +154,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -155,7 +178,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -451,20 +474,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{424E5EF4-563A-BB4B-A754-3D0CDD69DA25}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="89.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="48">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,167 +499,231 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
       <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
       <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
       <c r="D10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
       <c r="D12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
       <c r="D14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
       <c r="D16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
       <c r="D17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
       <c r="D18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
       <c r="D19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
       <c r="D20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
       <c r="D21" t="s">
-        <v>22</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>